<commit_message>
✅ Datos descarga actualizados y pesos
</commit_message>
<xml_diff>
--- a/aplicaciones/www/estaticos/datos/descarga/ya1-9-mortalidad-desnutricion-5.xlsx
+++ b/aplicaciones/www/estaticos/datos/descarga/ya1-9-mortalidad-desnutricion-5.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28224"/>
   <workbookPr/>
   <xr:revisionPtr revIDLastSave="0" documentId="11_61C6943C5D5F2B2225628E53C68C53F97AE0E11D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
@@ -10,10 +10,21 @@
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>

</xml_diff>